<commit_message>
import sics and fixtures for 2025
</commit_message>
<xml_diff>
--- a/scuelo/export_sics/External students.xlsx
+++ b/scuelo/export_sics/External students.xlsx
@@ -1,36 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enricosonno/Documents/ONLUS/00 Djicofè Gestione/00 DB relazionale/porting su SQL/AAA primo ambiente di sviluppo/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF883E9-F03B-C240-89DB-D46E267E8ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="16380" windowHeight="8200" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Classe" sheetId="1" r:id="rId1"/>
-    <sheet name="Scuole" sheetId="2" r:id="rId2"/>
-    <sheet name="Studente" sheetId="3" r:id="rId3"/>
+    <sheet name="Classe" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Scuole" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Studente" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Studente!$A$1:$T$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Studente!$A$1:$T$1</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr/>
   <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
-    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{D0CA8CA8-9F24-4464-BF8E-62219DCF47F9}"/>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="354">
   <si>
     <t>_PK_Classe_ID</t>
   </si>
@@ -473,7 +465,7 @@
     <t>Nome_Scuola</t>
   </si>
   <si>
-    <t>Ordine _Scuola</t>
+    <t xml:space="preserve">Ordine _Scuola</t>
   </si>
   <si>
     <t>Note_Scuola</t>
@@ -488,7 +480,7 @@
     <t>Sc_Nas_Mat</t>
   </si>
   <si>
-    <t>École Maternelle Centre social de Nasara</t>
+    <t xml:space="preserve">École Maternelle Centre social de Nasara</t>
   </si>
   <si>
     <t>Maternelle</t>
@@ -500,7 +492,7 @@
     <t>Sc_Nas_Pri</t>
   </si>
   <si>
-    <t>École primaire Centre social de Nasara</t>
+    <t xml:space="preserve">École primaire Centre social de Nasara</t>
   </si>
   <si>
     <t>Primaire</t>
@@ -509,7 +501,7 @@
     <t>Pri-Nas</t>
   </si>
   <si>
-    <t>Lycee Municipal de saaba</t>
+    <t xml:space="preserve">Lycee Municipal de saaba</t>
   </si>
   <si>
     <t>Lycée</t>
@@ -524,7 +516,7 @@
     <t>Lic-WLM</t>
   </si>
   <si>
-    <t>Lycee Provincial Molla Sanou de Bobo Dioulasso</t>
+    <t xml:space="preserve">Lycee Provincial Molla Sanou de Bobo Dioulasso</t>
   </si>
   <si>
     <t>Lic-LPMSBB</t>
@@ -536,13 +528,13 @@
     <t>Pri-WP</t>
   </si>
   <si>
-    <t>Ecole Primaire Catholique Effata Ludovic Pavoni</t>
+    <t xml:space="preserve">Ecole Primaire Catholique Effata Ludovic Pavoni</t>
   </si>
   <si>
     <t>Pri-EPCELP</t>
   </si>
   <si>
-    <t>Ecole Primaire Privé Les EMERITES</t>
+    <t xml:space="preserve">Ecole Primaire Privé Les EMERITES</t>
   </si>
   <si>
     <t>Pri-EPPLE</t>
@@ -554,7 +546,7 @@
     <t>Pri-YAMT</t>
   </si>
   <si>
-    <t>Ecole La Salle Badenya</t>
+    <t xml:space="preserve">Ecole La Salle Badenya</t>
   </si>
   <si>
     <t>Pri-LSB</t>
@@ -626,7 +618,7 @@
     <t>1408</t>
   </si>
   <si>
-    <t>Kabore Mouhaguidou</t>
+    <t xml:space="preserve">Kabore Mouhaguidou</t>
   </si>
   <si>
     <t>Mouhaguidou</t>
@@ -653,7 +645,7 @@
     <t>1415</t>
   </si>
   <si>
-    <t>Korgho Octave</t>
+    <t xml:space="preserve">Korgho Octave</t>
   </si>
   <si>
     <t>Octave</t>
@@ -665,7 +657,7 @@
     <t>1479</t>
   </si>
   <si>
-    <t>Kafando Carine</t>
+    <t xml:space="preserve">Kafando Carine</t>
   </si>
   <si>
     <t>Carine</t>
@@ -680,13 +672,13 @@
     <t>Bravo</t>
   </si>
   <si>
-    <t>ecole du village</t>
+    <t xml:space="preserve">ecole du village</t>
   </si>
   <si>
     <t>1497</t>
   </si>
   <si>
-    <t>Ouedraogo Mohamed</t>
+    <t xml:space="preserve">Ouedraogo Mohamed</t>
   </si>
   <si>
     <t>Mohamed</t>
@@ -695,13 +687,13 @@
     <t>Ouedraogo</t>
   </si>
   <si>
-    <t>ECOLE YAMTENGA</t>
+    <t xml:space="preserve">ECOLE YAMTENGA</t>
   </si>
   <si>
     <t>1590</t>
   </si>
   <si>
-    <t>Ilboudo Joel</t>
+    <t xml:space="preserve">Ilboudo Joel</t>
   </si>
   <si>
     <t>Joel</t>
@@ -713,16 +705,16 @@
     <t>1591</t>
   </si>
   <si>
-    <t>Kafando Salamata Kouka</t>
-  </si>
-  <si>
-    <t>Salamata Kouka</t>
+    <t xml:space="preserve">Kafando Salamata Kouka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salamata Kouka</t>
   </si>
   <si>
     <t>1592</t>
   </si>
   <si>
-    <t>Kiendrebeogo Elodie</t>
+    <t xml:space="preserve">Kiendrebeogo Elodie</t>
   </si>
   <si>
     <t>Elodie</t>
@@ -737,7 +729,7 @@
     <t>1593</t>
   </si>
   <si>
-    <t>Nacoulma Florentine</t>
+    <t xml:space="preserve">Nacoulma Florentine</t>
   </si>
   <si>
     <t>Florentine</t>
@@ -749,7 +741,7 @@
     <t>1594</t>
   </si>
   <si>
-    <t>Nana Fadilatou</t>
+    <t xml:space="preserve">Nana Fadilatou</t>
   </si>
   <si>
     <t>Fadilatou</t>
@@ -761,7 +753,7 @@
     <t>1595</t>
   </si>
   <si>
-    <t>Ouedraogo Faical</t>
+    <t xml:space="preserve">Ouedraogo Faical</t>
   </si>
   <si>
     <t>Faical</t>
@@ -770,7 +762,7 @@
     <t>1596</t>
   </si>
   <si>
-    <t>Ouedraogo Obed</t>
+    <t xml:space="preserve">Ouedraogo Obed</t>
   </si>
   <si>
     <t>Obed</t>
@@ -779,10 +771,10 @@
     <t>1597</t>
   </si>
   <si>
-    <t>Sam Abdoul Aquim</t>
-  </si>
-  <si>
-    <t>Abdoul Aquim</t>
+    <t xml:space="preserve">Sam Abdoul Aquim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abdoul Aquim</t>
   </si>
   <si>
     <t>Sam</t>
@@ -791,7 +783,7 @@
     <t>1598</t>
   </si>
   <si>
-    <t>Wangrawa Nadia</t>
+    <t xml:space="preserve">Wangrawa Nadia</t>
   </si>
   <si>
     <t>Nadia</t>
@@ -803,7 +795,7 @@
     <t>1599</t>
   </si>
   <si>
-    <t>Zoungrana Issa</t>
+    <t xml:space="preserve">Zoungrana Issa</t>
   </si>
   <si>
     <t>Issa</t>
@@ -815,10 +807,10 @@
     <t>1600</t>
   </si>
   <si>
-    <t>Congo Yacouba Robert</t>
-  </si>
-  <si>
-    <t>Yacouba Robert</t>
+    <t xml:space="preserve">Congo Yacouba Robert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yacouba Robert</t>
   </si>
   <si>
     <t>Congo</t>
@@ -830,7 +822,7 @@
     <t>1601</t>
   </si>
   <si>
-    <t>Kafando Salif</t>
+    <t xml:space="preserve">Kafando Salif</t>
   </si>
   <si>
     <t>Salif</t>
@@ -843,7 +835,7 @@
     <t>1602</t>
   </si>
   <si>
-    <t>Yameogo Alassane</t>
+    <t xml:space="preserve">Yameogo Alassane</t>
   </si>
   <si>
     <t>Alassane</t>
@@ -855,7 +847,7 @@
     <t>1603</t>
   </si>
   <si>
-    <t>Alantinga Anselme</t>
+    <t xml:space="preserve">Alantinga Anselme</t>
   </si>
   <si>
     <t>Anselme</t>
@@ -867,16 +859,16 @@
     <t>Extra</t>
   </si>
   <si>
-    <t>fille de Jean Baptiste</t>
+    <t xml:space="preserve">fille de Jean Baptiste</t>
   </si>
   <si>
     <t>1604</t>
   </si>
   <si>
-    <t>Compaore W.Rene Astrid</t>
-  </si>
-  <si>
-    <t>W.Rene Astrid</t>
+    <t xml:space="preserve">Compaore W.Rene Astrid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W.Rene Astrid</t>
   </si>
   <si>
     <t>Compaore</t>
@@ -885,7 +877,7 @@
     <t>1605</t>
   </si>
   <si>
-    <t>Dabone Angele</t>
+    <t xml:space="preserve">Dabone Angele</t>
   </si>
   <si>
     <t>Angele</t>
@@ -897,10 +889,10 @@
     <t>1606</t>
   </si>
   <si>
-    <t>Kabre Abdoul Nassirou</t>
-  </si>
-  <si>
-    <t>Abdoul Nassirou</t>
+    <t xml:space="preserve">Kabre Abdoul Nassirou</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abdoul Nassirou</t>
   </si>
   <si>
     <t>Kabre</t>
@@ -909,7 +901,7 @@
     <t>1607</t>
   </si>
   <si>
-    <t>Nikiema Tatiana</t>
+    <t xml:space="preserve">Nikiema Tatiana</t>
   </si>
   <si>
     <t>Tatiana</t>
@@ -921,19 +913,19 @@
     <t>1608</t>
   </si>
   <si>
-    <t>Sandwidi Tatiana</t>
+    <t xml:space="preserve">Sandwidi Tatiana</t>
   </si>
   <si>
     <t>Sandwidi</t>
   </si>
   <si>
-    <t>fille de Awa</t>
+    <t xml:space="preserve">fille de Awa</t>
   </si>
   <si>
     <t>1609</t>
   </si>
   <si>
-    <t>Sinare Mahamoudou</t>
+    <t xml:space="preserve">Sinare Mahamoudou</t>
   </si>
   <si>
     <t>Mahamoudou</t>
@@ -945,10 +937,10 @@
     <t>1610</t>
   </si>
   <si>
-    <t>Zangre Abdoul Rachid</t>
-  </si>
-  <si>
-    <t>Abdoul Rachid</t>
+    <t xml:space="preserve">Zangre Abdoul Rachid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abdoul Rachid</t>
   </si>
   <si>
     <t>Zangre</t>
@@ -957,65 +949,65 @@
     <t>1611</t>
   </si>
   <si>
-    <t>Zoungrana Ignace Wendpanga Olivier</t>
-  </si>
-  <si>
-    <t>Ignace Wendpanga Olivier</t>
-  </si>
-  <si>
-    <t>fille de Marguerite</t>
+    <t xml:space="preserve">Zoungrana Ignace Wendpanga Olivier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ignace Wendpanga Olivier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fille de Marguerite</t>
   </si>
   <si>
     <t>1612</t>
   </si>
   <si>
-    <t>Zoungrana Zenabo</t>
+    <t xml:space="preserve">Zoungrana Zenabo</t>
   </si>
   <si>
     <t>Zenabo</t>
   </si>
   <si>
-    <t>fille de Mahamadi</t>
+    <t xml:space="preserve">fille de Mahamadi</t>
   </si>
   <si>
     <t>1613</t>
   </si>
   <si>
-    <t>Nikiema Mahamadi</t>
+    <t xml:space="preserve">Nikiema Mahamadi</t>
   </si>
   <si>
     <t>Mahamadi</t>
   </si>
   <si>
-    <t>redouble
+    <t xml:space="preserve">redouble
 exclu de l'ecole pour mauvais conduite</t>
   </si>
   <si>
     <t>1614</t>
   </si>
   <si>
-    <t>Ilboudo Benewendé Naomie</t>
-  </si>
-  <si>
-    <t>Benewendé Naomie</t>
+    <t xml:space="preserve">Ilboudo Benewendé Naomie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benewendé Naomie</t>
   </si>
   <si>
     <t>1615</t>
   </si>
   <si>
-    <t>Ilboudo Wendkouni Simplice</t>
-  </si>
-  <si>
-    <t>Wendkouni Simplice</t>
+    <t xml:space="preserve">Ilboudo Wendkouni Simplice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wendkouni Simplice</t>
   </si>
   <si>
     <t>1616</t>
   </si>
   <si>
-    <t>Pafanam Natacha Erica</t>
-  </si>
-  <si>
-    <t>Natacha Erica</t>
+    <t xml:space="preserve">Pafanam Natacha Erica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Natacha Erica</t>
   </si>
   <si>
     <t>Pafanam</t>
@@ -1024,10 +1016,10 @@
     <t>1617</t>
   </si>
   <si>
-    <t>Sawadogo Mimtury Nemata</t>
-  </si>
-  <si>
-    <t>Mimtury Nemata</t>
+    <t xml:space="preserve">Sawadogo Mimtury Nemata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mimtury Nemata</t>
   </si>
   <si>
     <t>Sawadogo</t>
@@ -1036,7 +1028,7 @@
     <t>1618</t>
   </si>
   <si>
-    <t>Kiemtore Théophile</t>
+    <t xml:space="preserve">Kiemtore Théophile</t>
   </si>
   <si>
     <t>Théophile</t>
@@ -1048,7 +1040,7 @@
     <t>1619</t>
   </si>
   <si>
-    <t>Ouedraogo Yasmina</t>
+    <t xml:space="preserve">Ouedraogo Yasmina</t>
   </si>
   <si>
     <t>Yasmina</t>
@@ -1061,7 +1053,7 @@
     <t>1620</t>
   </si>
   <si>
-    <t>Compaore Adjaratou</t>
+    <t xml:space="preserve">Compaore Adjaratou</t>
   </si>
   <si>
     <t>Adjaratou</t>
@@ -1070,7 +1062,7 @@
     <t>1621</t>
   </si>
   <si>
-    <t>Koanda Pegwendé</t>
+    <t xml:space="preserve">Koanda Pegwendé</t>
   </si>
   <si>
     <t>Pegwendé</t>
@@ -1085,7 +1077,7 @@
     <t>1622</t>
   </si>
   <si>
-    <t>Ilboudou Mathias</t>
+    <t xml:space="preserve">Ilboudou Mathias</t>
   </si>
   <si>
     <t>Mathias</t>
@@ -1100,26 +1092,24 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
-      <sz val="10"/>
+      <sz val="10.000000"/>
+      <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
+      <sz val="10.000000"/>
+      <color indexed="64"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1128,42 +1118,72 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
+        <fgColor indexed="5"/>
+        <bgColor indexed="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="2"/>
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0"/>
+        <bgColor theme="9" tint="0"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="1">
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+  <cellXfs count="15">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="1" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf fontId="0" fillId="3" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf fontId="0" fillId="2" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="3" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1182,8 +1202,291 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Angsana New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Cordia New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1225,108 +1528,14 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:latin typeface="Calibri Light"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1334,7 +1543,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1360,7 +1569,7 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1412,16 +1621,28 @@
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -1437,7 +1658,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1468,26 +1689,19 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E60"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView topLeftCell="A24" zoomScale="140" workbookViewId="0">
+      <selection activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="25.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="25.1640625" defaultRowHeight="13"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" ht="14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1504,1012 +1718,1013 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="2" t="s">
+    <row r="3">
+      <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="4">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="2" t="s">
+    <row r="4">
+      <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="4">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="2" t="s">
+    <row r="5">
+      <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="4">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="2" t="s">
+    <row r="6">
+      <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="4">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A7" s="2" t="s">
+    <row r="7">
+      <c r="A7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="4">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8" s="2" t="s">
+    <row r="8">
+      <c r="A8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="4">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A9" s="2" t="s">
+    <row r="9">
+      <c r="A9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="4">
         <v>210</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A10" s="2" t="s">
+    <row r="10">
+      <c r="A10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="4">
         <v>211</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A11" s="2" t="s">
+    <row r="11">
+      <c r="A11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="4">
         <v>212</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A12" s="2" t="s">
+    <row r="12">
+      <c r="A12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="4">
         <v>213</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A13" s="2" t="s">
+    <row r="13">
+      <c r="A13" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="4">
         <v>214</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A14" s="2" t="s">
+    <row r="14">
+      <c r="A14" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="4">
         <v>215</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A15" s="2" t="s">
+    <row r="15">
+      <c r="A15" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="4">
         <v>216</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A16" s="2" t="s">
+    <row r="16">
+      <c r="A16" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="4">
         <v>310</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A17" s="2" t="s">
+    <row r="17">
+      <c r="A17" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="4">
         <v>311</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A18" s="2" t="s">
+    <row r="18">
+      <c r="A18" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="4">
         <v>312</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A19" s="2" t="s">
+    <row r="19">
+      <c r="A19" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="4">
         <v>313</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A20" s="2" t="s">
+    <row r="20">
+      <c r="A20" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="4">
         <v>314</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A21" s="2" t="s">
+    <row r="21">
+      <c r="A21" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="4">
         <v>315</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A22" s="2" t="s">
+    <row r="22">
+      <c r="A22" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="4">
         <v>316</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A23" s="2" t="s">
+    <row r="23">
+      <c r="A23" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="4">
         <v>410</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A24" s="2" t="s">
+    <row r="24">
+      <c r="A24" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="4">
         <v>411</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25" s="2" t="s">
+    <row r="25">
+      <c r="A25" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="4">
         <v>412</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26" s="2" t="s">
+    <row r="26">
+      <c r="A26" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="4">
         <v>413</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A27" s="2" t="s">
+    <row r="27">
+      <c r="A27" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27" s="4">
         <v>414</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A28" s="2" t="s">
+    <row r="28">
+      <c r="A28" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D28" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28" s="4">
         <v>415</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A29" s="2" t="s">
+    <row r="29">
+      <c r="A29" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D29" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E29" s="4">
         <v>416</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A30" s="2" t="s">
+    <row r="30">
+      <c r="A30" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D30" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E30" s="3">
+      <c r="E30" s="4">
         <v>510</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A31" s="2" t="s">
+    <row r="31">
+      <c r="A31" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E31" s="4">
         <v>511</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A32" s="2" t="s">
+    <row r="32">
+      <c r="A32" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D32" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E32" s="4">
         <v>512</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A33" s="2" t="s">
+    <row r="33">
+      <c r="A33" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="E33" s="3">
+      <c r="E33" s="4">
         <v>513</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A34" s="2" t="s">
+    <row r="34">
+      <c r="A34" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E34" s="3">
+      <c r="E34" s="4">
         <v>514</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A35" s="2" t="s">
+    <row r="35">
+      <c r="A35" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E35" s="3">
+      <c r="E35" s="4">
         <v>515</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A36" s="2" t="s">
+    <row r="36">
+      <c r="A36" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D36" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E36" s="3">
+      <c r="E36" s="4">
         <v>516</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A37" s="2" t="s">
+    <row r="37">
+      <c r="A37" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D37" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="E37" s="3">
+      <c r="E37" s="4">
         <v>604</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A38" s="2" t="s">
+    <row r="38">
+      <c r="A38" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D38" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="E38" s="3">
+      <c r="E38" s="4">
         <v>605</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A39" s="2" t="s">
+    <row r="39">
+      <c r="A39" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D39" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="E39" s="3">
+      <c r="E39" s="4">
         <v>606</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A40" s="2" t="s">
+    <row r="40">
+      <c r="A40" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D40" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E40" s="3">
+      <c r="E40" s="4">
         <v>607</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A41" s="2" t="s">
+    <row r="41">
+      <c r="A41" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D41" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="E41" s="3">
+      <c r="E41" s="4">
         <v>608</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A42" s="2" t="s">
+    <row r="42">
+      <c r="A42" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D42" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="E42" s="3">
+      <c r="E42" s="4">
         <v>609</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A43" s="2" t="s">
+    <row r="43">
+      <c r="A43" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C43" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D43" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="E43" s="3">
+      <c r="E43" s="4">
         <v>704</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A44" s="2" t="s">
+    <row r="44">
+      <c r="A44" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D44" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="E44" s="3">
+      <c r="E44" s="4">
         <v>705</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A45" s="2" t="s">
+    <row r="45">
+      <c r="A45" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D45" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="E45" s="3">
+      <c r="E45" s="4">
         <v>706</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A46" s="2" t="s">
+    <row r="46">
+      <c r="A46" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D46" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="E46" s="3">
+      <c r="E46" s="4">
         <v>707</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A47" s="2" t="s">
+    <row r="47">
+      <c r="A47" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D47" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="E47" s="3">
+      <c r="E47" s="4">
         <v>708</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A48" s="2" t="s">
+    <row r="48">
+      <c r="A48" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C48" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="D48" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="E48" s="3">
+      <c r="E48" s="4">
         <v>709</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A49" s="2" t="s">
+    <row r="49">
+      <c r="A49" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C49" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="D49" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E49" s="3">
+      <c r="E49" s="4">
         <v>804</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A50" s="2" t="s">
+    <row r="50">
+      <c r="A50" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C50" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="D50" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="E50" s="3">
+      <c r="E50" s="4">
         <v>805</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A51" s="2" t="s">
+    <row r="51">
+      <c r="A51" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C51" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="D51" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="E51" s="3">
+      <c r="E51" s="4">
         <v>806</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A52" s="2" t="s">
+    <row r="52">
+      <c r="A52" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B52" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C52" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D52" s="2" t="s">
+      <c r="D52" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="E52" s="3">
+      <c r="E52" s="4">
         <v>807</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A53" s="2" t="s">
+    <row r="53">
+      <c r="A53" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B53" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C53" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="D53" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="E53" s="3">
+      <c r="E53" s="4">
         <v>808</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A54" s="2" t="s">
+    <row r="54">
+      <c r="A54" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B54" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C54" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D54" s="2" t="s">
+      <c r="D54" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="E54" s="3">
+      <c r="E54" s="4">
         <v>809</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A55" s="2" t="s">
+    <row r="55">
+      <c r="A55" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B55" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="C55" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="D55" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="E55" s="3">
+      <c r="E55" s="4">
         <v>904</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A56" s="2" t="s">
+    <row r="56">
+      <c r="A56" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B56" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C56" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D56" s="2" t="s">
+      <c r="D56" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="E56" s="3">
+      <c r="E56" s="4">
         <v>905</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A57" s="2" t="s">
+    <row r="57">
+      <c r="A57" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B57" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C57" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D57" s="2" t="s">
+      <c r="D57" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="E57" s="3">
+      <c r="E57" s="4">
         <v>906</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A58" s="2" t="s">
+    <row r="58">
+      <c r="A58" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B58" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C58" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D58" s="2" t="s">
+      <c r="D58" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="E58" s="3">
+      <c r="E58" s="4">
         <v>907</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A59" s="2" t="s">
+    <row r="59">
+      <c r="A59" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B59" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C59" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D59" s="2" t="s">
+      <c r="D59" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="E59" s="3">
+      <c r="E59" s="4">
         <v>908</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A60" s="2" t="s">
+    <row r="60">
+      <c r="A60" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B60" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C60" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D60" s="2" t="s">
+      <c r="D60" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="E60" s="3">
+      <c r="E60" s="4">
         <v>909</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.78750000000000009" right="0.78750000000000009" top="1.05277777777778" bottom="1.05277777777778" header="0.78750000000000009" footer="0.78750000000000009"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="1" errors="displayed" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2518,26 +2733,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView topLeftCell="C1" zoomScale="140" workbookViewId="0">
+      <selection activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="25.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="25.1640625" defaultRowHeight="13"/>
   <cols>
-    <col min="2" max="2" width="55.33203125" customWidth="1"/>
-    <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="21.5" customWidth="1"/>
-    <col min="6" max="6" width="20.83203125" customWidth="1"/>
+    <col customWidth="1" min="2" max="2" width="55.33203125"/>
+    <col customWidth="1" min="3" max="3" width="21"/>
+    <col customWidth="1" min="4" max="4" width="21.5"/>
+    <col customWidth="1" min="6" max="6" width="20.83203125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" ht="14">
       <c r="A1" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>146</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -2553,196 +2767,197 @@
         <v>150</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A2" s="2" t="s">
+    <row r="2">
+      <c r="A2" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="4">
         <v>100</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3" s="2" t="s">
+    <row r="3">
+      <c r="A3" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="4">
         <v>100</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="3" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A4" s="2" t="s">
+    <row r="4">
+      <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="4">
         <v>200</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="3" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A5" s="2" t="s">
+    <row r="5">
+      <c r="A5" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="4">
         <v>300</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="3" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A6" s="2" t="s">
+    <row r="6">
+      <c r="A6" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="4">
         <v>400</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="3" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A7" s="2" t="s">
+    <row r="7">
+      <c r="A7" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="4">
         <v>500</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="3" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A8" s="2" t="s">
+    <row r="8">
+      <c r="A8" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="4">
         <v>600</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="3" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A9" s="2" t="s">
+    <row r="9">
+      <c r="A9" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="4">
         <v>700</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="3" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A10" s="2" t="s">
+    <row r="10">
+      <c r="A10" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="4">
         <v>800</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="3" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A11" s="2" t="s">
+    <row r="11">
+      <c r="A11" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="4">
         <v>900</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="3" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A12" s="2" t="s">
+    <row r="12">
+      <c r="A12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="4">
         <v>0</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="3" t="s">
         <v>176</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.78750000000000009" right="0.78750000000000009" top="1.05277777777778" bottom="1.05277777777778" header="0.78750000000000009" footer="0.78750000000000009"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2751,1278 +2966,1282 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:T38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView zoomScale="140" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="25.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="25.1640625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="3" max="3" width="37" customWidth="1"/>
-    <col min="19" max="19" width="49.6640625" customWidth="1"/>
+    <col min="1" max="1" style="6" width="25.1640625"/>
+    <col min="2" max="2" style="7" width="25.1640625"/>
+    <col customWidth="1" min="3" max="3" width="37"/>
+    <col customWidth="1" min="7" max="7" width="21.140625"/>
+    <col customWidth="1" min="8" max="8" width="8.8515625"/>
+    <col customWidth="1" min="19" max="19" width="49.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="14" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
+    <row r="1" s="8" customFormat="1" ht="13.5">
+      <c r="A1" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="9" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A2" s="2" t="s">
+    <row r="2">
+      <c r="A2" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="12">
         <v>41948</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="S2" s="3" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A3" s="2" t="s">
+    <row r="3">
+      <c r="A3" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="12">
         <v>41949</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="3" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A4" s="2" t="s">
+    <row r="4">
+      <c r="A4" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="12">
         <v>41587</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="S4" s="2" t="s">
+      <c r="S4" s="3" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A5" s="2" t="s">
+    <row r="5">
+      <c r="A5" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="12">
         <v>41400</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="S5" s="2" t="s">
+      <c r="S5" s="3" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A6" s="2" t="s">
+    <row r="6">
+      <c r="A6" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="12">
         <v>40902</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J6" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="O6" s="3">
+      <c r="O6" s="4">
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A7" s="2" t="s">
+    <row r="7">
+      <c r="A7" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="12">
         <v>42621</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="12">
         <v>40540</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J7" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="O7" s="3">
+      <c r="O7" s="4">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A8" s="2" t="s">
+    <row r="8">
+      <c r="A8" s="10" t="s">
         <v>229</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="12">
         <v>40161</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J8" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="O8" s="3">
+      <c r="O8" s="4">
         <v>33</v>
       </c>
-      <c r="S8" s="2" t="s">
+      <c r="S8" s="3" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A9" s="2" t="s">
+    <row r="9">
+      <c r="A9" s="10" t="s">
         <v>234</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="12">
         <v>42397</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="12">
         <v>40840</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" s="3" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A10" s="2" t="s">
+    <row r="10">
+      <c r="A10" s="10" t="s">
         <v>238</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="12">
         <v>42277</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="12">
         <v>40580</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="J10" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="O10" s="3">
+      <c r="O10" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A11" s="2" t="s">
+    <row r="11">
+      <c r="A11" s="10" t="s">
         <v>242</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="12">
         <v>41870</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="12">
         <v>40202</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="J11" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="O11" s="3">
+      <c r="O11" s="4">
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A12" s="2" t="s">
+    <row r="12">
+      <c r="A12" s="10" t="s">
         <v>245</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="I12" s="5">
+      <c r="I12" s="12">
         <v>40796</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="J12" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="O12" s="3">
+      <c r="O12" s="4">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A13" s="2" t="s">
+    <row r="13">
+      <c r="A13" s="10" t="s">
         <v>248</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="12">
         <v>42247</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H13" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="I13" s="5">
+      <c r="I13" s="12">
         <v>40838</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J13" s="3" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A14" s="2" t="s">
+    <row r="14">
+      <c r="A14" s="10" t="s">
         <v>252</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="12">
         <v>42619</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="I14" s="5">
+      <c r="I14" s="12">
         <v>40799</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="J14" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="O14" s="3">
+      <c r="O14" s="4">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A15" s="2" t="s">
+    <row r="15">
+      <c r="A15" s="10" t="s">
         <v>256</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H15" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="I15" s="5">
+      <c r="I15" s="12">
         <v>39889</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="J15" s="3" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A16" s="2" t="s">
+    <row r="16">
+      <c r="A16" s="10" t="s">
         <v>260</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H16" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="I16" s="5">
+      <c r="I16" s="12">
         <v>39933</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="J16" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="S16" s="2" t="s">
+      <c r="S16" s="3" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="28" x14ac:dyDescent="0.15">
-      <c r="A17" s="2" t="s">
+    <row r="17" ht="14.5" customHeight="1">
+      <c r="A17" s="10" t="s">
         <v>265</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H17" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="I17" s="5">
+      <c r="I17" s="12">
         <v>39800</v>
       </c>
-      <c r="J17" s="2" t="s">
+      <c r="J17" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="S17" s="6" t="s">
+      <c r="S17" s="13" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A18" s="2" t="s">
+    <row r="18">
+      <c r="A18" s="10" t="s">
         <v>269</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H18" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="I18" s="5">
+      <c r="I18" s="12">
         <v>39500</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="J18" s="3" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A19" s="2" t="s">
+    <row r="19">
+      <c r="A19" s="10" t="s">
         <v>273</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G19" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="H19" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="I19" s="5">
+      <c r="I19" s="12">
         <v>40288</v>
       </c>
-      <c r="J19" s="2" t="s">
+      <c r="J19" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="S19" s="2" t="s">
+      <c r="S19" s="3" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A20" s="2" t="s">
+    <row r="20">
+      <c r="A20" s="10" t="s">
         <v>279</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G20" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="H20" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="I20" s="5">
+      <c r="I20" s="12">
         <v>39740</v>
       </c>
-      <c r="J20" s="2" t="s">
+      <c r="J20" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="O20" s="3">
+      <c r="O20" s="4">
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A21" s="2" t="s">
+    <row r="21">
+      <c r="A21" s="10" t="s">
         <v>283</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="12">
         <v>41871</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G21" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="H21" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="I21" s="5">
+      <c r="I21" s="12">
         <v>40183</v>
       </c>
-      <c r="J21" s="2" t="s">
+      <c r="J21" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="O21" s="3">
+      <c r="O21" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A22" s="2" t="s">
+    <row r="22">
+      <c r="A22" s="10" t="s">
         <v>287</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="12">
         <v>41871</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E22" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F22" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="G22" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="H22" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="I22" s="5">
+      <c r="I22" s="12">
         <v>40456</v>
       </c>
-      <c r="J22" s="2" t="s">
+      <c r="J22" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="O22" s="3">
+      <c r="O22" s="4">
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A23" s="2" t="s">
+    <row r="23">
+      <c r="A23" s="10" t="s">
         <v>291</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E23" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F23" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G23" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="H23" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="I23" s="5">
+      <c r="I23" s="12">
         <v>40181</v>
       </c>
-      <c r="J23" s="2" t="s">
+      <c r="J23" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="O23" s="3">
+      <c r="O23" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A24" s="2" t="s">
+    <row r="24">
+      <c r="A24" s="10" t="s">
         <v>295</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F24" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G24" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="H24" s="2" t="s">
+      <c r="H24" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="I24" s="5">
+      <c r="I24" s="12">
         <v>40122</v>
       </c>
-      <c r="J24" s="2" t="s">
+      <c r="J24" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="O24" s="3">
+      <c r="O24" s="4">
         <v>52</v>
       </c>
-      <c r="S24" s="2" t="s">
+      <c r="S24" s="3" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A25" s="2" t="s">
+    <row r="25">
+      <c r="A25" s="10" t="s">
         <v>299</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="12">
         <v>41869</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="E25" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="G25" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="H25" s="2" t="s">
+      <c r="H25" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="I25" s="5">
+      <c r="I25" s="12">
         <v>40287</v>
       </c>
-      <c r="J25" s="2" t="s">
+      <c r="J25" s="3" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A26" s="2" t="s">
+    <row r="26">
+      <c r="A26" s="10" t="s">
         <v>303</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" s="12">
         <v>42248</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E26" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F26" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G26" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="H26" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="I26" s="5">
+      <c r="I26" s="12">
         <v>40317</v>
       </c>
-      <c r="J26" s="2" t="s">
+      <c r="J26" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="O26" s="3">
+      <c r="O26" s="4">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A27" s="2" t="s">
+    <row r="27">
+      <c r="A27" s="10" t="s">
         <v>307</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E27" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="F27" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="G27" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="H27" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="I27" s="5">
+      <c r="I27" s="12">
         <v>40468</v>
       </c>
-      <c r="J27" s="2" t="s">
+      <c r="J27" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="S27" s="2" t="s">
+      <c r="S27" s="3" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A28" s="2" t="s">
+    <row r="28">
+      <c r="A28" s="10" t="s">
         <v>311</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E28" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="F28" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="G28" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="H28" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="I28" s="5">
+      <c r="I28" s="12">
         <v>38630</v>
       </c>
-      <c r="J28" s="2" t="s">
+      <c r="J28" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="O28" s="3">
+      <c r="O28" s="4">
         <v>45</v>
       </c>
-      <c r="S28" s="2" t="s">
+      <c r="S28" s="3" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="28" x14ac:dyDescent="0.15">
-      <c r="A29" s="2" t="s">
+    <row r="29" ht="19.5" customHeight="1">
+      <c r="A29" s="10" t="s">
         <v>315</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="E29" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="F29" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="G29" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="H29" s="2" t="s">
+      <c r="H29" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="I29" s="5">
+      <c r="I29" s="12">
         <v>39727</v>
       </c>
-      <c r="J29" s="2" t="s">
+      <c r="J29" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="S29" s="6" t="s">
+      <c r="S29" s="13" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A30" s="2" t="s">
+    <row r="30">
+      <c r="A30" s="10" t="s">
         <v>319</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E30" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F30" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="G30" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="H30" s="2" t="s">
+      <c r="H30" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="I30" s="5">
+      <c r="I30" s="12">
         <v>40126</v>
       </c>
-      <c r="J30" s="2" t="s">
+      <c r="J30" s="3" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A31" s="2" t="s">
+    <row r="31">
+      <c r="A31" s="10" t="s">
         <v>322</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="E31" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="F31" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="G31" s="2" t="s">
+      <c r="G31" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="H31" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="I31" s="5">
+      <c r="I31" s="12">
         <v>39719</v>
       </c>
-      <c r="J31" s="2" t="s">
+      <c r="J31" s="3" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A32" s="2" t="s">
+    <row r="32">
+      <c r="A32" s="10" t="s">
         <v>325</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="E32" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F32" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="G32" s="2" t="s">
+      <c r="G32" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="H32" s="2" t="s">
+      <c r="H32" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="I32" s="5">
+      <c r="I32" s="12">
         <v>40054</v>
       </c>
-      <c r="J32" s="2" t="s">
+      <c r="J32" s="3" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A33" s="2" t="s">
+    <row r="33">
+      <c r="A33" s="10" t="s">
         <v>329</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="E33" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F33" s="3" t="s">
         <v>332</v>
       </c>
-      <c r="G33" s="2" t="s">
+      <c r="G33" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="H33" s="2" t="s">
+      <c r="H33" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="I33" s="5">
+      <c r="I33" s="12">
         <v>39803</v>
       </c>
-      <c r="J33" s="2" t="s">
+      <c r="J33" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="O33" s="3">
+      <c r="O33" s="4">
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A34" s="2" t="s">
+    <row r="34">
+      <c r="A34" s="10" t="s">
         <v>333</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="D34" s="5">
+      <c r="D34" s="12">
         <v>41870</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="E34" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="F34" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="G34" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="H34" s="2" t="s">
+      <c r="H34" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="I34" s="5">
+      <c r="I34" s="12">
         <v>39804</v>
       </c>
-      <c r="J34" s="2" t="s">
+      <c r="J34" s="3" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="28" x14ac:dyDescent="0.15">
-      <c r="A35" s="2" t="s">
+    <row r="35" ht="18.5" customHeight="1">
+      <c r="A35" s="10" t="s">
         <v>337</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="E35" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="F35" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="G35" s="2" t="s">
+      <c r="G35" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="H35" s="2" t="s">
+      <c r="H35" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="J35" s="2" t="s">
+      <c r="J35" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="S35" s="6" t="s">
+      <c r="S35" s="13" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A36" s="2" t="s">
+    <row r="36">
+      <c r="A36" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="E36" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="F36" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="G36" s="2" t="s">
+      <c r="G36" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="H36" s="2" t="s">
+      <c r="H36" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="I36" s="5">
+      <c r="I36" s="12">
         <v>39934</v>
       </c>
-      <c r="J36" s="2" t="s">
+      <c r="J36" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="O36" s="3">
+      <c r="O36" s="4">
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A37" s="2" t="s">
+    <row r="37">
+      <c r="A37" s="10" t="s">
         <v>344</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="E37" s="3" t="s">
         <v>346</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="F37" s="3" t="s">
         <v>347</v>
       </c>
-      <c r="G37" s="2" t="s">
+      <c r="G37" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="H37" s="2" t="s">
+      <c r="H37" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="I37" s="5">
+      <c r="I37" s="12">
         <v>39633</v>
       </c>
-      <c r="J37" s="2" t="s">
+      <c r="J37" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="S37" s="2" t="s">
+      <c r="S37" s="3" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A38" s="2" t="s">
+    <row r="38">
+      <c r="A38" s="14" t="s">
         <v>349</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="3" t="s">
         <v>350</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="E38" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="F38" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="G38" s="2" t="s">
+      <c r="G38" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="H38" s="2" t="s">
+      <c r="H38" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="J38" s="2" t="s">
+      <c r="J38" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="S38" s="2" t="s">
+      <c r="S38" s="3" t="s">
         <v>353</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:T1" xr:uid="{00000000-0001-0000-0200-000000000000}"/>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <autoFilter ref="A1:T1"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.78750000000000009" right="0.78750000000000009" top="1.05277777777778" bottom="1.05277777777778" header="0.78750000000000009" footer="0.78750000000000009"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>